<commit_message>
Upload de la imagen y archivo del diagrama de procesos, ademas del excel actualizado
</commit_message>
<xml_diff>
--- a/Calculo Mermelada.xlsx
+++ b/Calculo Mermelada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lilith\Desktop\Proyecto-Quimica-Mermelada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D88942-2DFE-4ED0-8FD4-28F835144E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D5F742-A35A-4610-B3F2-D2AF5DABC120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6DFA522A-53B6-478F-9D27-66162FDD3BAA}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>Manzanas Picadas</t>
   </si>
   <si>
-    <t>PROCESO 3 MOLIDO</t>
-  </si>
-  <si>
     <t>Desperdicio</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>PROCESO 3 MACHACADO</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A2:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,25 +547,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>19</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="I2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>13</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -636,13 +636,13 @@
         <v>331</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5" s="11" t="s">
         <v>1</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -686,25 +686,25 @@
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>16</v>
-      </c>
       <c r="D8" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>1</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -786,19 +786,19 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>16</v>
-      </c>
       <c r="D13" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -824,7 +824,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="3">
         <v>14</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3">
         <v>351</v>
@@ -870,24 +870,24 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>16</v>
-      </c>
       <c r="D18" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <f>B16</f>
@@ -908,7 +908,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="3">
         <f>B19/2</f>
@@ -932,7 +932,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="3">
         <v>325</v>
@@ -952,10 +952,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="C22" s="7">
         <f>(C19+C20)-C21</f>

</xml_diff>